<commit_message>
add new exercises, definitions, various updates
- updated various definitions. (see #144 for details)
- updated anki decks/wordlists with the above changes.
- added new definitions to the dictionary.
- added the following exercises.

# Lesson 22 (3rd ed.)
- Kanji Vocabulary: 記, 銀, and 回
- Kanji Vocabulary: 夕, 黒, and 用
- Kanji Vocabulary: 末, 待, and 残
- Kanji Vocabulary: 駅, 番, and 説
- Kanji Vocabulary: 案, 内, 忘, and 守
</commit_message>
<xml_diff>
--- a/resources/tools/wordlist_E-J/lessons-3rd/lesson-22.xlsx
+++ b/resources/tools/wordlist_E-J/lessons-3rd/lesson-22.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1117,6 +1117,810 @@
         </is>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>diary</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>日記|にっき</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>to fill in</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>記入する|きにゅうする</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>(news) article</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>記事|きじ</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>to memorize</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>暗記する|あんきする</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>bank</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>銀行|ぎんこう</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>silver medal</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>銀メダル|ぎんメダル</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>land covered with snow</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>銀世界|ぎんせかい</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>one time</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>一回|いっかい</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>out-of-service bus</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>回送バス|かいそうバス</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>last inning; last episode</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>最終回|さいしゅうかい</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>to turn</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>回す|まわす</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>evening</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>夕方|ゆうがた</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>dinner</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>夕食|ゆうしょく</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Tanabata</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>七夕|たなばた</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>setting sun</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>夕日|ゆうひ</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>evening newspaper</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>夕刊|ゆうかん</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Mr./Ms. Kuroki</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>黒木さん|くろきさん</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>black</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>黒い|くろい</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>black and white photograph</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>白黒写真|しろくろしゃしん</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>blackboard</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>黒板|こくばん</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>a thing to take care of</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>用事|ようじ</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>to prepare</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>用意する|よういする</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>for children</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>子供用|こどもよう</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>cost</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>費用|ひよう</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>weekend</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>週末|しゅうまつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>end of the month</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>月末|げつまつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>year-end</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>年末|ねんまつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>final examination</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>期末試験|きまつしけん</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>the end</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>末|すえ</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>to wait</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>待つ|まつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>waiting room</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>待合室|まちあいしつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>to expect</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>期待する|きたいする</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>invitation</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>招待|しょうたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>over-time work</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>残業|ざんぎょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>to leave</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>残す|のこす</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>regrettable</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>残念|ざんねん</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>regret</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>心残り|こころのこり</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>account balance</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>残高|ざんだか</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>station</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>駅|えき</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Tokyo Station</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>東京駅|とうきょうえき</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>train station attendant</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>駅員|えきいん</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>near/in front of the station</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>駅前|えきまえ</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>the first</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>一番|いちばん</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>番号|ばんごう</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>TV program</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>番組|ばんぐみ</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>police box</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>交番|こうばん</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>turn; order</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>順番|じゅんばん</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>to explain</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>説明する|せつめいする</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>novel</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>小説|しょうせつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>novelist</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>小説家|しょうせつか</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>to preach</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>説教する|せっきょうする</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>to guide</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>案内する|あんないする</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>information desk</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>案内所|あんないじょ</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>idea; proposal</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>案|あん</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>proposal</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>提案|ていあん</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>my wife</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>家内|かない</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>domestic</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>国内|こくない</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>internal medicine</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>内科|ないか</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>内側|うちがわ</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>to forget</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>忘れる|わすれる</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>lost article</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>忘れ物|わすれもの</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>year-end party</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>忘年会|ぼうねんかい</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>to keep (a promise)</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>守る|まもる</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>absence; not at home</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>留守|るす</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>answering machine</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>留守番電話|るすばんでんわ</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>charm</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>お守り|おまもり</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>security guard</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>守衛|しゅえい</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>